<commit_message>
Adjust error rate estimation
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -838,18 +838,8 @@
     <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="168" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -865,8 +855,18 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1248,7 +1248,7 @@
   <dimension ref="A1:DH24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="BT3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight"/>
@@ -1357,145 +1357,145 @@
       <c r="A1" s="41"/>
       <c r="B1" s="42"/>
       <c r="C1" s="37"/>
-      <c r="D1" s="92" t="s">
+      <c r="D1" s="90" t="s">
         <v>116</v>
       </c>
-      <c r="E1" s="92"/>
-      <c r="F1" s="92"/>
-      <c r="G1" s="92"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="90"/>
+      <c r="G1" s="90"/>
       <c r="H1" s="37"/>
-      <c r="I1" s="95" t="s">
+      <c r="I1" s="93" t="s">
         <v>74</v>
       </c>
-      <c r="J1" s="95"/>
-      <c r="K1" s="95"/>
-      <c r="L1" s="95"/>
-      <c r="M1" s="95"/>
-      <c r="N1" s="95"/>
-      <c r="O1" s="95"/>
-      <c r="P1" s="95"/>
-      <c r="Q1" s="95"/>
+      <c r="J1" s="93"/>
+      <c r="K1" s="93"/>
+      <c r="L1" s="93"/>
+      <c r="M1" s="93"/>
+      <c r="N1" s="93"/>
+      <c r="O1" s="93"/>
+      <c r="P1" s="93"/>
+      <c r="Q1" s="93"/>
       <c r="R1" s="34"/>
-      <c r="S1" s="91" t="s">
+      <c r="S1" s="89" t="s">
         <v>48</v>
       </c>
-      <c r="T1" s="91"/>
-      <c r="U1" s="91"/>
-      <c r="V1" s="91"/>
-      <c r="W1" s="91"/>
-      <c r="X1" s="91"/>
-      <c r="Y1" s="91"/>
-      <c r="Z1" s="91"/>
-      <c r="AA1" s="91"/>
-      <c r="AB1" s="91"/>
+      <c r="T1" s="89"/>
+      <c r="U1" s="89"/>
+      <c r="V1" s="89"/>
+      <c r="W1" s="89"/>
+      <c r="X1" s="89"/>
+      <c r="Y1" s="89"/>
+      <c r="Z1" s="89"/>
+      <c r="AA1" s="89"/>
+      <c r="AB1" s="89"/>
       <c r="AC1" s="36"/>
-      <c r="AD1" s="90" t="s">
+      <c r="AD1" s="97" t="s">
         <v>153</v>
       </c>
-      <c r="AE1" s="90"/>
-      <c r="AF1" s="90"/>
-      <c r="AG1" s="90"/>
-      <c r="AH1" s="90"/>
+      <c r="AE1" s="97"/>
+      <c r="AF1" s="97"/>
+      <c r="AG1" s="97"/>
+      <c r="AH1" s="97"/>
       <c r="AI1" s="36"/>
-      <c r="AJ1" s="88" t="s">
+      <c r="AJ1" s="95" t="s">
         <v>57</v>
       </c>
-      <c r="AK1" s="88"/>
+      <c r="AK1" s="95"/>
       <c r="AL1" s="39"/>
-      <c r="AM1" s="88" t="s">
+      <c r="AM1" s="95" t="s">
         <v>95</v>
       </c>
-      <c r="AN1" s="88"/>
-      <c r="AO1" s="88"/>
-      <c r="AP1" s="88"/>
-      <c r="AQ1" s="88"/>
+      <c r="AN1" s="95"/>
+      <c r="AO1" s="95"/>
+      <c r="AP1" s="95"/>
+      <c r="AQ1" s="95"/>
       <c r="AR1" s="39"/>
-      <c r="AS1" s="88" t="s">
+      <c r="AS1" s="95" t="s">
         <v>58</v>
       </c>
-      <c r="AT1" s="88"/>
-      <c r="AU1" s="88"/>
-      <c r="AV1" s="88"/>
+      <c r="AT1" s="95"/>
+      <c r="AU1" s="95"/>
+      <c r="AV1" s="95"/>
       <c r="AW1" s="36"/>
-      <c r="AX1" s="89" t="s">
+      <c r="AX1" s="94" t="s">
         <v>127</v>
       </c>
-      <c r="AY1" s="89"/>
-      <c r="AZ1" s="89"/>
-      <c r="BA1" s="89"/>
+      <c r="AY1" s="94"/>
+      <c r="AZ1" s="94"/>
+      <c r="BA1" s="94"/>
       <c r="BB1" s="36"/>
-      <c r="BC1" s="89" t="s">
+      <c r="BC1" s="94" t="s">
         <v>122</v>
       </c>
-      <c r="BD1" s="89"/>
-      <c r="BE1" s="89"/>
-      <c r="BF1" s="89"/>
-      <c r="BG1" s="89"/>
-      <c r="BH1" s="89"/>
-      <c r="BI1" s="89"/>
-      <c r="BJ1" s="89"/>
-      <c r="BK1" s="89"/>
+      <c r="BD1" s="94"/>
+      <c r="BE1" s="94"/>
+      <c r="BF1" s="94"/>
+      <c r="BG1" s="94"/>
+      <c r="BH1" s="94"/>
+      <c r="BI1" s="94"/>
+      <c r="BJ1" s="94"/>
+      <c r="BK1" s="94"/>
       <c r="BL1" s="36"/>
-      <c r="BM1" s="94" t="s">
+      <c r="BM1" s="92" t="s">
         <v>128</v>
       </c>
-      <c r="BN1" s="94"/>
-      <c r="BO1" s="94"/>
+      <c r="BN1" s="92"/>
+      <c r="BO1" s="92"/>
       <c r="BP1" s="36"/>
-      <c r="BQ1" s="94" t="s">
+      <c r="BQ1" s="92" t="s">
         <v>129</v>
       </c>
-      <c r="BR1" s="94"/>
-      <c r="BS1" s="94"/>
-      <c r="BT1" s="94"/>
-      <c r="BU1" s="94"/>
-      <c r="BV1" s="94"/>
-      <c r="BW1" s="94"/>
-      <c r="BX1" s="94"/>
-      <c r="BY1" s="94"/>
-      <c r="BZ1" s="94"/>
-      <c r="CA1" s="94"/>
+      <c r="BR1" s="92"/>
+      <c r="BS1" s="92"/>
+      <c r="BT1" s="92"/>
+      <c r="BU1" s="92"/>
+      <c r="BV1" s="92"/>
+      <c r="BW1" s="92"/>
+      <c r="BX1" s="92"/>
+      <c r="BY1" s="92"/>
+      <c r="BZ1" s="92"/>
+      <c r="CA1" s="92"/>
       <c r="CB1" s="36"/>
-      <c r="CC1" s="94" t="s">
+      <c r="CC1" s="92" t="s">
         <v>120</v>
       </c>
-      <c r="CD1" s="94"/>
-      <c r="CE1" s="94"/>
-      <c r="CF1" s="94"/>
-      <c r="CG1" s="94"/>
-      <c r="CH1" s="94"/>
-      <c r="CI1" s="94"/>
-      <c r="CJ1" s="94"/>
+      <c r="CD1" s="92"/>
+      <c r="CE1" s="92"/>
+      <c r="CF1" s="92"/>
+      <c r="CG1" s="92"/>
+      <c r="CH1" s="92"/>
+      <c r="CI1" s="92"/>
+      <c r="CJ1" s="92"/>
       <c r="CK1" s="36"/>
-      <c r="CL1" s="93" t="s">
+      <c r="CL1" s="91" t="s">
         <v>71</v>
       </c>
-      <c r="CM1" s="93"/>
-      <c r="CN1" s="93"/>
-      <c r="CO1" s="93"/>
-      <c r="CP1" s="93"/>
+      <c r="CM1" s="91"/>
+      <c r="CN1" s="91"/>
+      <c r="CO1" s="91"/>
+      <c r="CP1" s="91"/>
       <c r="CQ1" s="36"/>
-      <c r="CR1" s="87" t="s">
+      <c r="CR1" s="96" t="s">
         <v>123</v>
       </c>
-      <c r="CS1" s="87"/>
-      <c r="CT1" s="87"/>
-      <c r="CU1" s="87"/>
-      <c r="CV1" s="87"/>
-      <c r="CW1" s="87"/>
-      <c r="CX1" s="87"/>
-      <c r="CY1" s="87"/>
+      <c r="CS1" s="96"/>
+      <c r="CT1" s="96"/>
+      <c r="CU1" s="96"/>
+      <c r="CV1" s="96"/>
+      <c r="CW1" s="96"/>
+      <c r="CX1" s="96"/>
+      <c r="CY1" s="96"/>
       <c r="CZ1" s="36"/>
-      <c r="DA1" s="87" t="s">
+      <c r="DA1" s="96" t="s">
         <v>119</v>
       </c>
-      <c r="DB1" s="87"/>
-      <c r="DC1" s="87"/>
-      <c r="DD1" s="87"/>
-      <c r="DE1" s="87"/>
-      <c r="DF1" s="87"/>
-      <c r="DG1" s="87"/>
-      <c r="DH1" s="87"/>
+      <c r="DB1" s="96"/>
+      <c r="DC1" s="96"/>
+      <c r="DD1" s="96"/>
+      <c r="DE1" s="96"/>
+      <c r="DF1" s="96"/>
+      <c r="DG1" s="96"/>
+      <c r="DH1" s="96"/>
     </row>
     <row r="2" spans="1:112" s="2" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -1956,7 +1956,7 @@
       <c r="AZ3" s="8">
         <v>250139</v>
       </c>
-      <c r="BA3" s="96">
+      <c r="BA3" s="87">
         <v>0</v>
       </c>
       <c r="BB3" s="36"/>
@@ -1984,7 +1984,7 @@
       <c r="BJ3" s="8">
         <v>348718</v>
       </c>
-      <c r="BK3" s="96">
+      <c r="BK3" s="87">
         <v>0</v>
       </c>
       <c r="BL3" s="36"/>
@@ -2091,10 +2091,10 @@
       <c r="CW3" s="29">
         <v>5390971</v>
       </c>
-      <c r="CX3" s="97">
+      <c r="CX3" s="88">
         <v>8.0679999999999988E-3</v>
       </c>
-      <c r="CY3" s="97">
+      <c r="CY3" s="88">
         <v>3.4860000000000004E-3</v>
       </c>
       <c r="CZ3" s="36"/>
@@ -2116,10 +2116,10 @@
       <c r="DF3" s="29">
         <v>5344447</v>
       </c>
-      <c r="DG3" s="97">
+      <c r="DG3" s="88">
         <v>6.7730000000000004E-3</v>
       </c>
-      <c r="DH3" s="97">
+      <c r="DH3" s="88">
         <v>3.3679999999999999E-3</v>
       </c>
     </row>
@@ -2274,7 +2274,7 @@
       <c r="AZ4" s="8">
         <v>250138</v>
       </c>
-      <c r="BA4" s="96">
+      <c r="BA4" s="87">
         <v>1.9999999999999999E-6</v>
       </c>
       <c r="BB4" s="36"/>
@@ -2302,7 +2302,7 @@
       <c r="BJ4" s="8">
         <v>348718</v>
       </c>
-      <c r="BK4" s="96">
+      <c r="BK4" s="87">
         <v>0</v>
       </c>
       <c r="BL4" s="36"/>
@@ -2409,10 +2409,10 @@
       <c r="CW4" s="29">
         <v>5337172</v>
       </c>
-      <c r="CX4" s="97">
+      <c r="CX4" s="88">
         <v>9.4669999999999997E-3</v>
       </c>
-      <c r="CY4" s="97">
+      <c r="CY4" s="88">
         <v>4.4050000000000001E-3</v>
       </c>
       <c r="CZ4" s="36"/>
@@ -2434,10 +2434,10 @@
       <c r="DF4" s="29">
         <v>5343419</v>
       </c>
-      <c r="DG4" s="97">
+      <c r="DG4" s="88">
         <v>7.986E-3</v>
       </c>
-      <c r="DH4" s="97">
+      <c r="DH4" s="88">
         <v>4.2529999999999998E-3</v>
       </c>
     </row>
@@ -2592,7 +2592,7 @@
       <c r="AZ5" s="8">
         <v>101183</v>
       </c>
-      <c r="BA5" s="96">
+      <c r="BA5" s="87">
         <v>0</v>
       </c>
       <c r="BB5" s="36"/>
@@ -2620,7 +2620,7 @@
       <c r="BJ5" s="8">
         <v>163014</v>
       </c>
-      <c r="BK5" s="96">
+      <c r="BK5" s="87">
         <v>0</v>
       </c>
       <c r="BL5" s="36"/>
@@ -2727,10 +2727,10 @@
       <c r="CW5" s="29">
         <v>4653773</v>
       </c>
-      <c r="CX5" s="97">
+      <c r="CX5" s="88">
         <v>1.4985999999999999E-2</v>
       </c>
-      <c r="CY5" s="97">
+      <c r="CY5" s="88">
         <v>8.7760000000000008E-3</v>
       </c>
       <c r="CZ5" s="36"/>
@@ -2752,10 +2752,10 @@
       <c r="DF5" s="29">
         <v>5356696</v>
       </c>
-      <c r="DG5" s="97">
+      <c r="DG5" s="88">
         <v>1.1952000000000001E-2</v>
       </c>
-      <c r="DH5" s="97">
+      <c r="DH5" s="88">
         <v>8.234E-3</v>
       </c>
     </row>
@@ -2910,7 +2910,7 @@
       <c r="AZ6" s="8">
         <v>117385</v>
       </c>
-      <c r="BA6" s="96">
+      <c r="BA6" s="87">
         <v>0</v>
       </c>
       <c r="BB6" s="36"/>
@@ -2938,7 +2938,7 @@
       <c r="BJ6" s="8">
         <v>188481</v>
       </c>
-      <c r="BK6" s="96">
+      <c r="BK6" s="87">
         <v>0</v>
       </c>
       <c r="BL6" s="36"/>
@@ -3045,10 +3045,10 @@
       <c r="CW6" s="29">
         <v>2284274</v>
       </c>
-      <c r="CX6" s="97">
+      <c r="CX6" s="88">
         <v>1.6677999999999998E-2</v>
       </c>
-      <c r="CY6" s="97">
+      <c r="CY6" s="88">
         <v>1.0725999999999999E-2</v>
       </c>
       <c r="CZ6" s="36"/>
@@ -3070,10 +3070,10 @@
       <c r="DF6" s="29">
         <v>4979475</v>
       </c>
-      <c r="DG6" s="97">
+      <c r="DG6" s="88">
         <v>1.2963000000000001E-2</v>
       </c>
-      <c r="DH6" s="97">
+      <c r="DH6" s="88">
         <v>9.5239999999999995E-3</v>
       </c>
     </row>
@@ -3228,7 +3228,7 @@
       <c r="AZ7" s="8">
         <v>247434</v>
       </c>
-      <c r="BA7" s="96">
+      <c r="BA7" s="87">
         <v>0</v>
       </c>
       <c r="BB7" s="36"/>
@@ -3256,7 +3256,7 @@
       <c r="BJ7" s="8">
         <v>376128</v>
       </c>
-      <c r="BK7" s="96">
+      <c r="BK7" s="87">
         <v>0</v>
       </c>
       <c r="BL7" s="36"/>
@@ -3363,10 +3363,10 @@
       <c r="CW7" s="29">
         <v>5553946</v>
       </c>
-      <c r="CX7" s="97">
+      <c r="CX7" s="88">
         <v>1.2286999999999999E-2</v>
       </c>
-      <c r="CY7" s="97">
+      <c r="CY7" s="88">
         <v>6.4640000000000001E-3</v>
       </c>
       <c r="CZ7" s="36"/>
@@ -3388,10 +3388,10 @@
       <c r="DF7" s="29">
         <v>5584078</v>
       </c>
-      <c r="DG7" s="97">
+      <c r="DG7" s="88">
         <v>1.0043999999999999E-2</v>
       </c>
-      <c r="DH7" s="97">
+      <c r="DH7" s="88">
         <v>6.1050000000000002E-3</v>
       </c>
     </row>
@@ -3546,7 +3546,7 @@
       <c r="AZ8" s="8">
         <v>225799</v>
       </c>
-      <c r="BA8" s="96">
+      <c r="BA8" s="87">
         <v>1.9999999999999999E-6</v>
       </c>
       <c r="BB8" s="36"/>
@@ -3574,7 +3574,7 @@
       <c r="BJ8" s="8">
         <v>376127</v>
       </c>
-      <c r="BK8" s="96">
+      <c r="BK8" s="87">
         <v>0</v>
       </c>
       <c r="BL8" s="36"/>
@@ -3681,10 +3681,10 @@
       <c r="CW8" s="29">
         <v>2999032</v>
       </c>
-      <c r="CX8" s="97">
+      <c r="CX8" s="88">
         <v>1.1545000000000001E-2</v>
       </c>
-      <c r="CY8" s="97">
+      <c r="CY8" s="88">
         <v>6.0109999999999999E-3</v>
       </c>
       <c r="CZ8" s="36"/>
@@ -3706,10 +3706,10 @@
       <c r="DF8" s="29">
         <v>5360772</v>
       </c>
-      <c r="DG8" s="97">
+      <c r="DG8" s="88">
         <v>1.0184E-2</v>
       </c>
-      <c r="DH8" s="97">
+      <c r="DH8" s="88">
         <v>5.7189999999999993E-3</v>
       </c>
     </row>
@@ -3864,7 +3864,7 @@
       <c r="AZ9" s="8">
         <v>326008</v>
       </c>
-      <c r="BA9" s="96">
+      <c r="BA9" s="87">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="BB9" s="36"/>
@@ -3892,7 +3892,7 @@
       <c r="BJ9" s="8">
         <v>335272</v>
       </c>
-      <c r="BK9" s="96">
+      <c r="BK9" s="87">
         <v>0</v>
       </c>
       <c r="BL9" s="36"/>
@@ -3999,10 +3999,10 @@
       <c r="CW9" s="29">
         <v>5305856</v>
       </c>
-      <c r="CX9" s="97">
+      <c r="CX9" s="88">
         <v>9.9439999999999997E-3</v>
       </c>
-      <c r="CY9" s="97">
+      <c r="CY9" s="88">
         <v>5.744E-3</v>
       </c>
       <c r="CZ9" s="36"/>
@@ -4024,10 +4024,10 @@
       <c r="DF9" s="29">
         <v>5317165</v>
       </c>
-      <c r="DG9" s="97">
+      <c r="DG9" s="88">
         <v>8.9420000000000003E-3</v>
       </c>
-      <c r="DH9" s="97">
+      <c r="DH9" s="88">
         <v>5.6959999999999997E-3</v>
       </c>
     </row>
@@ -4182,7 +4182,7 @@
       <c r="AZ10" s="8">
         <v>350656</v>
       </c>
-      <c r="BA10" s="96">
+      <c r="BA10" s="87">
         <v>3.9999999999999998E-6</v>
       </c>
       <c r="BB10" s="36"/>
@@ -4210,7 +4210,7 @@
       <c r="BJ10" s="8">
         <v>412960</v>
       </c>
-      <c r="BK10" s="96">
+      <c r="BK10" s="87">
         <v>0</v>
       </c>
       <c r="BL10" s="36"/>
@@ -4317,10 +4317,10 @@
       <c r="CW10" s="29">
         <v>5303005</v>
       </c>
-      <c r="CX10" s="97">
+      <c r="CX10" s="88">
         <v>1.1310000000000001E-2</v>
       </c>
-      <c r="CY10" s="97">
+      <c r="CY10" s="88">
         <v>5.5360000000000001E-3</v>
       </c>
       <c r="CZ10" s="36"/>
@@ -4342,10 +4342,10 @@
       <c r="DF10" s="29">
         <v>5383727</v>
       </c>
-      <c r="DG10" s="97">
+      <c r="DG10" s="88">
         <v>9.9990000000000009E-3</v>
       </c>
-      <c r="DH10" s="97">
+      <c r="DH10" s="88">
         <v>5.189E-3</v>
       </c>
     </row>
@@ -4500,7 +4500,7 @@
       <c r="AZ11" s="8">
         <v>148459</v>
       </c>
-      <c r="BA11" s="96">
+      <c r="BA11" s="87">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="BB11" s="36"/>
@@ -4528,7 +4528,7 @@
       <c r="BJ11" s="8">
         <v>251072</v>
       </c>
-      <c r="BK11" s="96">
+      <c r="BK11" s="87">
         <v>0</v>
       </c>
       <c r="BL11" s="36"/>
@@ -4635,10 +4635,10 @@
       <c r="CW11" s="29">
         <v>5342912</v>
       </c>
-      <c r="CX11" s="97">
+      <c r="CX11" s="88">
         <v>1.8835999999999999E-2</v>
       </c>
-      <c r="CY11" s="97">
+      <c r="CY11" s="88">
         <v>1.2319999999999999E-2</v>
       </c>
       <c r="CZ11" s="36"/>
@@ -4660,10 +4660,10 @@
       <c r="DF11" s="29">
         <v>1092219</v>
       </c>
-      <c r="DG11" s="97">
+      <c r="DG11" s="88">
         <v>1.4028000000000001E-2</v>
       </c>
-      <c r="DH11" s="97">
+      <c r="DH11" s="88">
         <v>1.0343E-2</v>
       </c>
     </row>
@@ -4818,7 +4818,7 @@
       <c r="AZ12" s="8">
         <v>174882</v>
       </c>
-      <c r="BA12" s="96">
+      <c r="BA12" s="87">
         <v>0</v>
       </c>
       <c r="BB12" s="36"/>
@@ -4846,7 +4846,7 @@
       <c r="BJ12" s="8">
         <v>198467</v>
       </c>
-      <c r="BK12" s="96">
+      <c r="BK12" s="87">
         <v>0</v>
       </c>
       <c r="BL12" s="36"/>
@@ -4953,10 +4953,10 @@
       <c r="CW12" s="29">
         <v>5178122</v>
       </c>
-      <c r="CX12" s="97">
+      <c r="CX12" s="88">
         <v>8.9639999999999997E-3</v>
       </c>
-      <c r="CY12" s="97">
+      <c r="CY12" s="88">
         <v>3.5570000000000003E-3</v>
       </c>
       <c r="CZ12" s="36"/>
@@ -4978,10 +4978,10 @@
       <c r="DF12" s="29">
         <v>5249042</v>
       </c>
-      <c r="DG12" s="97">
+      <c r="DG12" s="88">
         <v>8.0479999999999996E-3</v>
       </c>
-      <c r="DH12" s="97">
+      <c r="DH12" s="88">
         <v>3.3839999999999999E-3</v>
       </c>
     </row>
@@ -5136,7 +5136,7 @@
       <c r="AZ13" s="8">
         <v>109907</v>
       </c>
-      <c r="BA13" s="96">
+      <c r="BA13" s="87">
         <v>0</v>
       </c>
       <c r="BB13" s="36"/>
@@ -5164,7 +5164,7 @@
       <c r="BJ13" s="8">
         <v>163015</v>
       </c>
-      <c r="BK13" s="96">
+      <c r="BK13" s="87">
         <v>0</v>
       </c>
       <c r="BL13" s="36"/>
@@ -5271,10 +5271,10 @@
       <c r="CW13" s="29">
         <v>4807134</v>
       </c>
-      <c r="CX13" s="97">
+      <c r="CX13" s="88">
         <v>1.2621E-2</v>
       </c>
-      <c r="CY13" s="97">
+      <c r="CY13" s="88">
         <v>6.7979999999999994E-3</v>
       </c>
       <c r="CZ13" s="36"/>
@@ -5296,10 +5296,10 @@
       <c r="DF13" s="29">
         <v>5298548</v>
       </c>
-      <c r="DG13" s="97">
+      <c r="DG13" s="88">
         <v>1.0410999999999998E-2</v>
       </c>
-      <c r="DH13" s="97">
+      <c r="DH13" s="88">
         <v>6.0929999999999995E-3</v>
       </c>
     </row>
@@ -5454,7 +5454,7 @@
       <c r="AZ14" s="8">
         <v>319758</v>
       </c>
-      <c r="BA14" s="96">
+      <c r="BA14" s="87">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="BB14" s="36"/>
@@ -5482,7 +5482,7 @@
       <c r="BJ14" s="8">
         <v>361802</v>
       </c>
-      <c r="BK14" s="96">
+      <c r="BK14" s="87">
         <v>0</v>
       </c>
       <c r="BL14" s="36"/>
@@ -5589,10 +5589,10 @@
       <c r="CW14" s="29">
         <v>5256073</v>
       </c>
-      <c r="CX14" s="97">
+      <c r="CX14" s="88">
         <v>1.1916E-2</v>
       </c>
-      <c r="CY14" s="97">
+      <c r="CY14" s="88">
         <v>6.3460000000000009E-3</v>
       </c>
       <c r="CZ14" s="36"/>
@@ -5614,10 +5614,10 @@
       <c r="DF14" s="29">
         <v>5277423</v>
       </c>
-      <c r="DG14" s="97">
+      <c r="DG14" s="88">
         <v>1.0634999999999999E-2</v>
       </c>
-      <c r="DH14" s="97">
+      <c r="DH14" s="88">
         <v>6.058E-3</v>
       </c>
     </row>
@@ -5821,7 +5821,7 @@
         <f>AVERAGE(AZ$3:AZ$14)</f>
         <v>218479</v>
       </c>
-      <c r="BA16" s="96">
+      <c r="BA16" s="87">
         <f>AVERAGE(BA$3:BA$14)</f>
         <v>9.1666666666666664E-7</v>
       </c>
@@ -5851,7 +5851,7 @@
         <f t="shared" si="12"/>
         <v>293647.83333333331</v>
       </c>
-      <c r="BK16" s="96">
+      <c r="BK16" s="87">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -5938,11 +5938,11 @@
         <f t="shared" si="14"/>
         <v>4784355.833333333</v>
       </c>
-      <c r="CX16" s="97">
+      <c r="CX16" s="88">
         <f t="shared" si="14"/>
         <v>1.22185E-2</v>
       </c>
-      <c r="CY16" s="97">
+      <c r="CY16" s="88">
         <f t="shared" si="14"/>
         <v>6.6807500000000001E-3</v>
       </c>
@@ -5959,11 +5959,11 @@
         <f>AVERAGE(DF$3:DF$14)</f>
         <v>4965584.25</v>
       </c>
-      <c r="DG16" s="97">
+      <c r="DG16" s="88">
         <f>AVERAGE(DG$3:DG$14)</f>
         <v>1.0163749999999999E-2</v>
       </c>
-      <c r="DH16" s="97">
+      <c r="DH16" s="88">
         <f>AVERAGE(DH$3:DH$14)</f>
         <v>6.1638333333333328E-3</v>
       </c>
@@ -6564,6 +6564,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="DA1:DH1"/>
+    <mergeCell ref="CR1:CY1"/>
+    <mergeCell ref="AM1:AQ1"/>
+    <mergeCell ref="AX1:BA1"/>
+    <mergeCell ref="AD1:AH1"/>
     <mergeCell ref="S1:AB1"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="CL1:CP1"/>
@@ -6574,11 +6579,6 @@
     <mergeCell ref="AS1:AV1"/>
     <mergeCell ref="BM1:BO1"/>
     <mergeCell ref="BQ1:CA1"/>
-    <mergeCell ref="DA1:DH1"/>
-    <mergeCell ref="CR1:CY1"/>
-    <mergeCell ref="AM1:AQ1"/>
-    <mergeCell ref="AX1:BA1"/>
-    <mergeCell ref="AD1:AH1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>